<commit_message>
finished importation with progress bar
</commit_message>
<xml_diff>
--- a/public/templates/UW_SurveyProgram_Import.xlsx
+++ b/public/templates/UW_SurveyProgram_Import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\almeida\repos\MARE\UVC-api\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDC292C-B2B1-4C88-BD52-EF99A41763EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF842B81-D77A-4785-92F3-151147E81CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{13F33F4D-E77F-4168-A6AC-0D4C829D8FE1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{13F33F4D-E77F-4168-A6AC-0D4C829D8FE1}"/>
   </bookViews>
   <sheets>
     <sheet name="DIVE_SITE_METADATA" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>SAMPLE#</t>
   </si>
@@ -48,15 +48,9 @@
     <t>Locality</t>
   </si>
   <si>
-    <t>L#</t>
-  </si>
-  <si>
     <t>Site</t>
   </si>
   <si>
-    <t>Site#</t>
-  </si>
-  <si>
     <t>Daily_Dive#</t>
   </si>
   <si>
@@ -102,9 +96,6 @@
     <t>Distance</t>
   </si>
   <si>
-    <t>Functions:</t>
-  </si>
-  <si>
     <t>[FUNCTION_A]</t>
   </si>
   <si>
@@ -135,9 +126,6 @@
     <t>Phylum</t>
   </si>
   <si>
-    <t>Indicators:</t>
-  </si>
-  <si>
     <t>[INDICATOR_A]</t>
   </si>
   <si>
@@ -154,6 +142,21 @@
   </si>
   <si>
     <t>Ntotal</t>
+  </si>
+  <si>
+    <t>Locality Code</t>
+  </si>
+  <si>
+    <t>Site Code</t>
+  </si>
+  <si>
+    <t>Surveyed area</t>
+  </si>
+  <si>
+    <t>Indicators</t>
+  </si>
+  <si>
+    <t>Functions</t>
   </si>
 </sst>
 </file>
@@ -576,7 +579,7 @@
   <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,9 +587,9 @@
     <col min="1" max="1" width="31.28515625" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
@@ -607,70 +610,70 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -703,16 +706,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -728,7 +731,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,25 +743,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -771,10 +774,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,30 +785,34 @@
     <col min="1" max="1" width="26.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="39.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -821,7 +828,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,25 +843,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>